<commit_message>
added a verry rough estimate of some of my work hours, there is maybe some tasks missing for trello
</commit_message>
<xml_diff>
--- a/manual/worksheet.xlsx
+++ b/manual/worksheet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\joarbels\projects\let-me-out\manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7144F59D-D277-1C4C-9357-FE6944FBC23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB9A376-D7B1-43A2-93D0-B7AD9A109733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Hours</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Comment each others sections constructively</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -678,22 +681,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA831349-0FC3-5540-B36A-3848ABED492D}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.69921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="69.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -704,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -712,31 +715,40 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -744,7 +756,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -752,23 +764,29 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C8" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -776,23 +794,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -800,23 +824,29 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -824,7 +854,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -832,7 +862,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -840,7 +870,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -848,15 +878,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+      <c r="C20" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -864,7 +897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -872,7 +905,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -880,47 +913,62 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C24" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="C25" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C27" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C28" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -928,7 +976,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -936,7 +984,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -944,7 +992,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -952,7 +1000,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -960,7 +1008,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -968,7 +1016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -976,7 +1024,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="43" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -984,7 +1032,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="27" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -992,15 +1040,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="29" x14ac:dyDescent="0.2">
+      <c r="C38" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1008,7 +1059,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1016,7 +1067,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1024,7 +1075,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
@@ -1032,23 +1083,29 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C43" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C44" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
@@ -1056,15 +1113,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C46" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>72</v>
       </c>
@@ -1072,7 +1132,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>73</v>
       </c>
@@ -1080,28 +1140,43 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C49" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>63</v>
+      </c>
+      <c r="C51" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="1">
+        <f>SUM(C2:C51)</f>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Worksheet] MR adding elements and time
</commit_message>
<xml_diff>
--- a/manual/worksheet.xlsx
+++ b/manual/worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\joarbels\projects\let-me-out\manual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiterm/Programing/AAU/let-me-out/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB9A376-D7B1-43A2-93D0-B7AD9A109733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FA0CE6-4954-D341-894F-2DB8F62D4640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>Hours</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Fixing overleaf template</t>
   </si>
   <si>
-    <t>Make GitHub repository</t>
-  </si>
-  <si>
     <t>Make a Database in Postgres</t>
   </si>
   <si>
@@ -276,6 +273,12 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>Isn't it the automated thing we do everyday? So basically no time from us, but the scripts are working instead</t>
+  </si>
+  <si>
+    <t>Create scrpt to fetch blocked Ips</t>
   </si>
 </sst>
 </file>
@@ -681,150 +684,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA831349-0FC3-5540-B36A-3848ABED492D}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.69921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="69.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -835,348 +844,357 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C20" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="27" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="B38" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="B40" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="B43" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="B49" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C52" s="1">
         <f>SUM(C2:C51)</f>
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[worksheet] Correcting the worksheet, add everyones name.
</commit_message>
<xml_diff>
--- a/manual/worksheet.xlsx
+++ b/manual/worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiterm/Programing/AAU/let-me-out/manual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FA0CE6-4954-D341-894F-2DB8F62D4640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F443485-7C6E-C648-A218-D9496A790246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
+    <workbookView xWindow="0" yWindow="1460" windowWidth="28800" windowHeight="16040" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t>Hours</t>
   </si>
@@ -279,13 +279,37 @@
   </si>
   <si>
     <t>Create scrpt to fetch blocked Ips</t>
+  </si>
+  <si>
+    <t>Joar</t>
+  </si>
+  <si>
+    <t>Márton</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Cho</t>
+  </si>
+  <si>
+    <t>Rifat</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Gergely</t>
+  </si>
+  <si>
+    <t>WORKING HOUR PER MEMBER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,6 +338,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -329,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -352,11 +391,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -368,6 +418,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -684,517 +744,887 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA831349-0FC3-5540-B36A-3848ABED492D}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="69.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="6" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="C2" s="6">
+        <f>SUM(D2:J2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C51" si="0">SUM(D3:J3)</f>
+        <v>20</v>
+      </c>
+      <c r="D3" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D7" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="C9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C12" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D13" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="E14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="C15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="C16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="6">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D20" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="E20" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="C21" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="C22" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C23" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E24" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="6">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="D25" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="E25" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E26" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="6">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="D27" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E27" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="6">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D28" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E28" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C29" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C30" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C31" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C32" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C33" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C34" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="43" x14ac:dyDescent="0.2">
+      <c r="C35" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="43" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="C36" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C37" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D38" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="E38" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C39" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C40" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="C42" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D43" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E43" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D44" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E44" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C45" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D46" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E46" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="C47" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="6">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D49" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E49" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D50" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D51" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C52" s="1">
+      <c r="E51" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6">
         <f>SUM(C2:C51)</f>
+        <v>360</v>
+      </c>
+      <c r="D52" s="6">
+        <f t="shared" ref="D52:J52" si="1">SUM(D2:D51)</f>
+        <v>173</v>
+      </c>
+      <c r="E52" s="6">
+        <f t="shared" si="1"/>
         <v>187</v>
+      </c>
+      <c r="F52" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H52" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[worksheet] Upload the hours for Gery
</commit_message>
<xml_diff>
--- a/manual/worksheet.xlsx
+++ b/manual/worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F443485-7C6E-C648-A218-D9496A790246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A209FBD-20F8-0044-AF0D-A7921569F9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1460" windowWidth="28800" windowHeight="16040" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
+    <workbookView xWindow="6160" yWindow="900" windowWidth="21980" windowHeight="16040" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Hours</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>WORKING HOUR PER MEMBER</t>
+  </si>
+  <si>
+    <t>Help others: to understand networking basics and with their asks</t>
+  </si>
+  <si>
+    <t>Investigate delisting methods for blocklists</t>
   </si>
 </sst>
 </file>
@@ -406,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -428,6 +434,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -744,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA831349-0FC3-5540-B36A-3848ABED492D}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -806,6 +815,9 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="J2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -816,13 +828,16 @@
       </c>
       <c r="C3" s="6">
         <f t="shared" ref="C3:C51" si="0">SUM(D3:J3)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -834,13 +849,16 @@
       </c>
       <c r="C4" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -852,12 +870,15 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
     </row>
@@ -874,6 +895,9 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+      <c r="J6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -884,13 +908,16 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1">
         <v>16</v>
       </c>
       <c r="E7" s="1">
         <v>16</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="85" x14ac:dyDescent="0.2">
@@ -910,6 +937,9 @@
       <c r="E8" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -924,6 +954,9 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
+      <c r="J9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -942,6 +975,9 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -952,12 +988,15 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11">
         <v>1</v>
       </c>
     </row>
@@ -970,10 +1009,13 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
+      <c r="J12">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -984,13 +1026,16 @@
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1002,13 +1047,16 @@
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
+      </c>
+      <c r="J14">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -1024,6 +1072,9 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
+      <c r="J15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1034,12 +1085,15 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1047,15 +1101,18 @@
         <v>57</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>SUM(D17:J17)</f>
+        <v>6</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1064,12 +1121,15 @@
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>80</v>
       </c>
@@ -1084,8 +1144,11 @@
       <c r="E19" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="43" x14ac:dyDescent="0.2">
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1094,7 +1157,7 @@
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1">
         <v>25</v>
@@ -1102,8 +1165,11 @@
       <c r="E20" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1112,12 +1178,15 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1126,12 +1195,15 @@
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1140,12 +1212,15 @@
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -1162,8 +1237,11 @@
       <c r="E24" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1172,7 +1250,7 @@
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D25" s="1">
         <v>28</v>
@@ -1180,8 +1258,11 @@
       <c r="E25" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1190,7 +1271,7 @@
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
@@ -1198,8 +1279,11 @@
       <c r="E26" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1216,8 +1300,11 @@
       <c r="E27" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1234,8 +1321,11 @@
       <c r="E28" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -1248,8 +1338,11 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -1262,8 +1355,11 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1276,8 +1372,11 @@
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -1290,8 +1389,11 @@
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -1300,12 +1402,15 @@
       </c>
       <c r="C33" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -1318,8 +1423,11 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -1328,12 +1436,15 @@
       </c>
       <c r="C35" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="43" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1346,8 +1457,11 @@
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -1356,12 +1470,15 @@
       </c>
       <c r="C37" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -1378,8 +1495,11 @@
       <c r="E38" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -1392,8 +1512,11 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -1406,8 +1529,11 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -1422,8 +1548,11 @@
       <c r="E41" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -1432,12 +1561,15 @@
       </c>
       <c r="C42" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -1446,7 +1578,7 @@
       </c>
       <c r="C43" s="6">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D43" s="1">
         <v>6</v>
@@ -1454,8 +1586,11 @@
       <c r="E43" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>69</v>
       </c>
@@ -1464,7 +1599,7 @@
       </c>
       <c r="C44" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D44" s="1">
         <v>8</v>
@@ -1472,8 +1607,11 @@
       <c r="E44" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
@@ -1486,8 +1624,11 @@
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -1496,7 +1637,7 @@
       </c>
       <c r="C46" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D46" s="1">
         <v>4</v>
@@ -1504,8 +1645,11 @@
       <c r="E46" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -1518,8 +1662,11 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -1528,12 +1675,15 @@
       </c>
       <c r="C48" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1">
         <v>3</v>
       </c>
+      <c r="J48">
+        <v>6</v>
+      </c>
     </row>
     <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -1544,13 +1694,16 @@
       </c>
       <c r="C49" s="6">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D49" s="1">
         <v>6</v>
       </c>
       <c r="E49" s="1">
         <v>6</v>
+      </c>
+      <c r="J49">
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1570,6 +1723,9 @@
       <c r="E50" s="1">
         <v>1</v>
       </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
@@ -1579,8 +1735,8 @@
         <v>62</v>
       </c>
       <c r="C51" s="6">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>SUM(D51:J51)</f>
+        <v>16</v>
       </c>
       <c r="D51" s="1">
         <v>4</v>
@@ -1588,43 +1744,82 @@
       <c r="E51" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+      <c r="J51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6">
-        <f>SUM(C2:C51)</f>
-        <v>360</v>
-      </c>
-      <c r="D52" s="6">
-        <f t="shared" ref="D52:J52" si="1">SUM(D2:D51)</f>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6">
+        <f>SUM(C2:C53)</f>
+        <v>570</v>
+      </c>
+      <c r="D54" s="6">
+        <f t="shared" ref="C54:I54" si="1">SUM(D2:D53)</f>
         <v>173</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E54" s="6">
         <f t="shared" si="1"/>
         <v>187</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F54" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G54" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H54" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I52" s="6">
+      <c r="I54" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J52" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="J54" s="6">
+        <f>SUM(J2:J53)</f>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[worksheet] Jonas hours upload
</commit_message>
<xml_diff>
--- a/manual/worksheet.xlsx
+++ b/manual/worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A209FBD-20F8-0044-AF0D-A7921569F9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6434C0-35AC-D24A-9FB0-520FE5A1E167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6160" yWindow="900" windowWidth="21980" windowHeight="16040" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -434,9 +434,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -755,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA831349-0FC3-5540-B36A-3848ABED492D}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,10 +808,13 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(D2:J2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
       <c r="J2">
         <v>0</v>
       </c>
@@ -827,13 +827,16 @@
         <v>50</v>
       </c>
       <c r="C3" s="6">
-        <f t="shared" ref="C3:C51" si="0">SUM(D3:J3)</f>
-        <v>40</v>
+        <f t="shared" ref="C3:C50" si="0">SUM(D3:J3)</f>
+        <v>50</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
       </c>
       <c r="E3" s="1">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1">
         <v>10</v>
       </c>
       <c r="J3">
@@ -849,13 +852,16 @@
       </c>
       <c r="C4" s="6">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -870,13 +876,16 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -891,10 +900,13 @@
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
       <c r="J6">
         <v>0</v>
       </c>
@@ -908,13 +920,16 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1">
         <v>16</v>
       </c>
       <c r="E7" s="1">
         <v>16</v>
+      </c>
+      <c r="I7" s="1">
+        <v>10</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -929,13 +944,16 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>79</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -950,10 +968,13 @@
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
+      <c r="I9" s="1">
+        <v>10</v>
+      </c>
       <c r="J9">
         <v>0</v>
       </c>
@@ -975,6 +996,7 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
+      <c r="I10" s="1"/>
       <c r="J10">
         <v>0</v>
       </c>
@@ -988,13 +1010,16 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1013,6 +1038,7 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12">
         <v>7</v>
       </c>
@@ -1034,6 +1060,7 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
+      <c r="I13" s="1"/>
       <c r="J13">
         <v>1</v>
       </c>
@@ -1055,6 +1082,7 @@
       <c r="E14" s="1">
         <v>2</v>
       </c>
+      <c r="I14" s="1"/>
       <c r="J14">
         <v>11</v>
       </c>
@@ -1068,10 +1096,13 @@
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
+      <c r="I15" s="1">
+        <v>10</v>
+      </c>
       <c r="J15">
         <v>0</v>
       </c>
@@ -1085,10 +1116,13 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
+      <c r="I16" s="1">
+        <v>10</v>
+      </c>
       <c r="J16">
         <v>15</v>
       </c>
@@ -1102,11 +1136,14 @@
       </c>
       <c r="C17" s="6">
         <f>SUM(D17:J17)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
         <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>10</v>
       </c>
       <c r="J17">
         <v>5</v>
@@ -1125,6 +1162,7 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
+      <c r="I18" s="6"/>
       <c r="J18">
         <v>1</v>
       </c>
@@ -1144,6 +1182,7 @@
       <c r="E19" s="1">
         <v>5</v>
       </c>
+      <c r="I19" s="1"/>
       <c r="J19" s="1">
         <v>0</v>
       </c>
@@ -1165,6 +1204,7 @@
       <c r="E20" s="1">
         <v>25</v>
       </c>
+      <c r="I20" s="1"/>
       <c r="J20">
         <v>7</v>
       </c>
@@ -1178,10 +1218,13 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
+      <c r="I21" s="1">
+        <v>30</v>
+      </c>
       <c r="J21">
         <v>6</v>
       </c>
@@ -1199,6 +1242,7 @@
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
+      <c r="I22" s="1"/>
       <c r="J22">
         <v>18</v>
       </c>
@@ -1216,6 +1260,7 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
+      <c r="I23" s="1"/>
       <c r="J23">
         <v>8</v>
       </c>
@@ -1237,6 +1282,7 @@
       <c r="E24" s="1">
         <v>6</v>
       </c>
+      <c r="I24" s="1"/>
       <c r="J24">
         <v>0</v>
       </c>
@@ -1250,13 +1296,16 @@
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="D25" s="1">
         <v>28</v>
       </c>
       <c r="E25" s="1">
         <v>28</v>
+      </c>
+      <c r="I25" s="1">
+        <v>30</v>
       </c>
       <c r="J25">
         <v>11</v>
@@ -1271,13 +1320,16 @@
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
       <c r="E26" s="1">
         <v>2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>10</v>
       </c>
       <c r="J26">
         <v>3</v>
@@ -1292,13 +1344,16 @@
       </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="D27" s="1">
         <v>28</v>
       </c>
       <c r="E27" s="1">
         <v>28</v>
+      </c>
+      <c r="I27" s="1">
+        <v>30</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -1321,6 +1376,7 @@
       <c r="E28" s="1">
         <v>16</v>
       </c>
+      <c r="I28" s="1"/>
       <c r="J28">
         <v>0</v>
       </c>
@@ -1338,6 +1394,7 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
+      <c r="I29" s="1"/>
       <c r="J29">
         <v>0</v>
       </c>
@@ -1355,6 +1412,7 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
+      <c r="I30" s="1"/>
       <c r="J30">
         <v>0</v>
       </c>
@@ -1372,6 +1430,7 @@
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
+      <c r="I31" s="1"/>
       <c r="J31">
         <v>0</v>
       </c>
@@ -1389,6 +1448,7 @@
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
+      <c r="I32" s="1"/>
       <c r="J32">
         <v>0</v>
       </c>
@@ -1402,10 +1462,13 @@
       </c>
       <c r="C33" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
+      <c r="I33" s="1">
+        <v>5</v>
+      </c>
       <c r="J33">
         <v>4</v>
       </c>
@@ -1423,6 +1486,7 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
+      <c r="I34" s="1"/>
       <c r="J34">
         <v>0</v>
       </c>
@@ -1440,6 +1504,7 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="J35">
         <v>12</v>
       </c>
@@ -1457,6 +1522,7 @@
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
+      <c r="I36" s="1"/>
       <c r="J36">
         <v>0</v>
       </c>
@@ -1470,10 +1536,13 @@
       </c>
       <c r="C37" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
+      <c r="I37" s="1">
+        <v>10</v>
+      </c>
       <c r="J37">
         <v>16</v>
       </c>
@@ -1487,13 +1556,16 @@
       </c>
       <c r="C38" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D38" s="1">
         <v>4</v>
       </c>
       <c r="E38" s="1">
         <v>4</v>
+      </c>
+      <c r="I38" s="1">
+        <v>10</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -1512,6 +1584,7 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
+      <c r="I39" s="1"/>
       <c r="J39">
         <v>0</v>
       </c>
@@ -1529,6 +1602,7 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
+      <c r="I40" s="1"/>
       <c r="J40">
         <v>0</v>
       </c>
@@ -1548,6 +1622,7 @@
       <c r="E41" s="1">
         <v>5</v>
       </c>
+      <c r="I41" s="1"/>
       <c r="J41">
         <v>0</v>
       </c>
@@ -1565,6 +1640,7 @@
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
+      <c r="I42" s="1"/>
       <c r="J42">
         <v>8</v>
       </c>
@@ -1578,13 +1654,16 @@
       </c>
       <c r="C43" s="6">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D43" s="1">
         <v>6</v>
       </c>
       <c r="E43" s="1">
         <v>6</v>
+      </c>
+      <c r="I43" s="1">
+        <v>10</v>
       </c>
       <c r="J43">
         <v>13</v>
@@ -1607,6 +1686,7 @@
       <c r="E44" s="1">
         <v>8</v>
       </c>
+      <c r="I44" s="1"/>
       <c r="J44">
         <v>4</v>
       </c>
@@ -1620,10 +1700,13 @@
       </c>
       <c r="C45" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
+      <c r="I45" s="1">
+        <v>1</v>
+      </c>
       <c r="J45">
         <v>0</v>
       </c>
@@ -1637,13 +1720,16 @@
       </c>
       <c r="C46" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D46" s="1">
         <v>4</v>
       </c>
       <c r="E46" s="1">
         <v>4</v>
+      </c>
+      <c r="I46" s="1">
+        <v>10</v>
       </c>
       <c r="J46">
         <v>8</v>
@@ -1658,10 +1744,13 @@
       </c>
       <c r="C47" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
       <c r="J47">
         <v>0</v>
       </c>
@@ -1681,6 +1770,7 @@
       <c r="E48" s="1">
         <v>3</v>
       </c>
+      <c r="I48" s="1"/>
       <c r="J48">
         <v>6</v>
       </c>
@@ -1694,13 +1784,16 @@
       </c>
       <c r="C49" s="6">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D49" s="1">
         <v>6</v>
       </c>
       <c r="E49" s="1">
         <v>6</v>
+      </c>
+      <c r="I49" s="1">
+        <v>20</v>
       </c>
       <c r="J49">
         <v>12</v>
@@ -1723,6 +1816,7 @@
       <c r="E50" s="1">
         <v>1</v>
       </c>
+      <c r="I50" s="1"/>
       <c r="J50">
         <v>0</v>
       </c>
@@ -1736,13 +1830,16 @@
       </c>
       <c r="C51" s="6">
         <f>SUM(D51:J51)</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D51" s="1">
         <v>4</v>
       </c>
       <c r="E51" s="1">
         <v>4</v>
+      </c>
+      <c r="I51" s="1">
+        <v>5</v>
       </c>
       <c r="J51">
         <v>8</v>
@@ -1752,7 +1849,7 @@
       <c r="A52" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C52" s="6"/>
@@ -1762,7 +1859,7 @@
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
-      <c r="J52" s="9">
+      <c r="J52" s="1">
         <v>20</v>
       </c>
     </row>
@@ -1770,7 +1867,7 @@
       <c r="A53" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C53" s="6"/>
@@ -1780,7 +1877,7 @@
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
-      <c r="J53" s="9">
+      <c r="J53" s="1">
         <v>8</v>
       </c>
     </row>
@@ -1791,10 +1888,10 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6">
         <f>SUM(C2:C53)</f>
-        <v>570</v>
+        <v>818</v>
       </c>
       <c r="D54" s="6">
-        <f t="shared" ref="C54:I54" si="1">SUM(D2:D53)</f>
+        <f t="shared" ref="D54:I54" si="1">SUM(D2:D53)</f>
         <v>173</v>
       </c>
       <c r="E54" s="6">
@@ -1815,7 +1912,7 @@
       </c>
       <c r="I54" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="J54" s="6">
         <f>SUM(J2:J53)</f>

</xml_diff>

<commit_message>
[worksheet] Update hours of Rasmus
</commit_message>
<xml_diff>
--- a/manual/worksheet.xlsx
+++ b/manual/worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choeun/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F028AEEB-98C1-884E-8E4B-6A3CF4516993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D98316-5960-D34D-B269-5BD430FA2AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
   <si>
     <t>Hours</t>
   </si>
@@ -309,17 +309,20 @@
   </si>
   <si>
     <t>Investigate delisting methods for blocklists</t>
+  </si>
+  <si>
+    <t>Rasmus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -327,7 +330,7 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -340,14 +343,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -355,16 +358,23 @@
       <b/>
       <sz val="20"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -419,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -443,9 +453,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -461,7 +473,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -757,24 +769,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA831349-0FC3-5540-B36A-3848ABED492D}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="88" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="69.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="69.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31">
+    <row r="1" spans="1:11" ht="27" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -805,8 +818,11 @@
       <c r="J1" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="19">
+      <c r="K1" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -825,8 +841,11 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="38">
+      <c r="K2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -855,8 +874,11 @@
       <c r="J3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="38">
+      <c r="K3" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -885,8 +907,11 @@
       <c r="J4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="38">
+      <c r="K4" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -915,8 +940,11 @@
       <c r="J5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="19">
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -935,8 +963,11 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="19">
+      <c r="K6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -959,8 +990,11 @@
       <c r="J7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="95">
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -983,8 +1017,11 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="44">
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="43" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1003,8 +1040,11 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="19">
+      <c r="K9" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -1031,8 +1071,11 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="38">
+      <c r="K10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1061,8 +1104,11 @@
       <c r="J11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="44">
+      <c r="K11" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="43" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1082,8 +1128,11 @@
       <c r="J12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="19">
+      <c r="K12" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1107,8 +1156,9 @@
       <c r="J13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="19">
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1129,8 +1179,11 @@
       <c r="J14">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="19">
+      <c r="K14" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1152,8 +1205,9 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="30">
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1172,8 +1226,9 @@
       <c r="J16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="19">
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1194,8 +1249,11 @@
       <c r="J17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="19">
+      <c r="K17" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1212,8 +1270,9 @@
       <c r="J18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="19">
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>80</v>
       </c>
@@ -1232,8 +1291,9 @@
       <c r="J19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="30">
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" ht="43" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1257,8 +1317,11 @@
       <c r="J20">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="19">
+      <c r="K20" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1277,8 +1340,11 @@
       <c r="J21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="19">
+      <c r="K21" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="29" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1295,8 +1361,11 @@
       <c r="J22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="30">
+      <c r="K22" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1313,8 +1382,9 @@
       <c r="J23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="19">
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -1335,8 +1405,11 @@
       <c r="J24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="19">
+      <c r="K24" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1359,8 +1432,9 @@
       <c r="J25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="38">
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1389,8 +1463,11 @@
       <c r="J26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="19">
+      <c r="K26" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1413,8 +1490,9 @@
       <c r="J27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="19">
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1438,8 +1516,9 @@
       <c r="J28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="19">
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -1456,8 +1535,11 @@
       <c r="J29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="19">
+      <c r="K29" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -1474,8 +1556,11 @@
       <c r="J30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="19">
+      <c r="K30" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1498,8 +1583,11 @@
       <c r="J31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="19">
+      <c r="K31" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -1519,8 +1607,11 @@
       <c r="J32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="19">
+      <c r="K32" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -1539,8 +1630,9 @@
       <c r="J33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="19">
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -1560,8 +1652,9 @@
       <c r="J34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="19">
+      <c r="K34" s="9"/>
+    </row>
+    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -1578,8 +1671,9 @@
       <c r="J35">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="30">
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="1:11" ht="43" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1599,8 +1693,9 @@
       <c r="J36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="30">
+      <c r="K36" s="9"/>
+    </row>
+    <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -1619,8 +1714,9 @@
       <c r="J37">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="19">
+      <c r="K37" s="9"/>
+    </row>
+    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -1643,8 +1739,9 @@
       <c r="J38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="19">
+      <c r="K38" s="9"/>
+    </row>
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -1664,8 +1761,11 @@
       <c r="J39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="19">
+      <c r="K39" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -1685,8 +1785,11 @@
       <c r="J40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="19">
+      <c r="K40" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -1705,8 +1808,9 @@
       <c r="J41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="19">
+      <c r="K41" s="9"/>
+    </row>
+    <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -1723,8 +1827,9 @@
       <c r="J42">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="38">
+      <c r="K42" s="9"/>
+    </row>
+    <row r="43" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -1753,8 +1858,11 @@
       <c r="J43">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="19">
+      <c r="K43" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>69</v>
       </c>
@@ -1775,8 +1883,9 @@
       <c r="J44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="19">
+      <c r="K44" s="9"/>
+    </row>
+    <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
@@ -1795,8 +1904,11 @@
       <c r="J45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="19">
+      <c r="K45" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -1819,8 +1931,9 @@
       <c r="J46">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="19">
+      <c r="K46" s="9"/>
+    </row>
+    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>71</v>
       </c>
@@ -1842,8 +1955,9 @@
       <c r="J47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="19">
+      <c r="K47" s="9"/>
+    </row>
+    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>72</v>
       </c>
@@ -1862,8 +1976,9 @@
       <c r="J48">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="19">
+      <c r="K48" s="9"/>
+    </row>
+    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>73</v>
       </c>
@@ -1886,8 +2001,9 @@
       <c r="J49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="19">
+      <c r="K49" s="9"/>
+    </row>
+    <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
@@ -1908,8 +2024,9 @@
       <c r="J50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="38">
+      <c r="K50" s="9"/>
+    </row>
+    <row r="51" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>77</v>
       </c>
@@ -1938,8 +2055,11 @@
       <c r="J51">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" s="7" customFormat="1" ht="38">
+      <c r="K51" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="7" customFormat="1" ht="35" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>89</v>
       </c>
@@ -1956,8 +2076,9 @@
       <c r="J52" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" s="7" customFormat="1" ht="19">
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="1:11" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>90</v>
       </c>
@@ -1974,8 +2095,9 @@
       <c r="J53" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" s="7" customFormat="1" ht="19">
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="1:11" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>88</v>
       </c>
@@ -2011,6 +2133,10 @@
       <c r="J54" s="6">
         <f>SUM(J2:J53)</f>
         <v>238</v>
+      </c>
+      <c r="K54" s="6">
+        <f>SUM(K2:K53)</f>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[worksheet] Update hours of Rifat
</commit_message>
<xml_diff>
--- a/manual/worksheet.xlsx
+++ b/manual/worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D98316-5960-D34D-B269-5BD430FA2AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A53C1C7-C509-E841-8E7F-FF814BB19E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
   </bookViews>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA831349-0FC3-5540-B36A-3848ABED492D}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="88" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
@@ -1456,6 +1456,9 @@
       </c>
       <c r="G26">
         <v>5</v>
+      </c>
+      <c r="H26">
+        <v>9</v>
       </c>
       <c r="I26" s="1">
         <v>10</v>
@@ -1527,10 +1530,13 @@
       </c>
       <c r="C29" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
+      <c r="H29">
+        <v>15</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29">
         <v>0</v>
@@ -1548,10 +1554,13 @@
       </c>
       <c r="C30" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
+      <c r="H30">
+        <v>12</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30">
         <v>0</v>
@@ -1682,12 +1691,15 @@
       </c>
       <c r="C36" s="6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="G36">
         <v>10</v>
+      </c>
+      <c r="H36">
+        <v>25</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36">
@@ -1838,7 +1850,7 @@
       </c>
       <c r="C43" s="6">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D43" s="1">
         <v>6</v>
@@ -1850,6 +1862,9 @@
         <v>13</v>
       </c>
       <c r="G43">
+        <v>11</v>
+      </c>
+      <c r="H43">
         <v>11</v>
       </c>
       <c r="I43" s="1">
@@ -2035,7 +2050,7 @@
       </c>
       <c r="C51" s="6">
         <f>SUM(D51:J51)</f>
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D51" s="1">
         <v>4</v>
@@ -2048,6 +2063,9 @@
       </c>
       <c r="G51">
         <v>5</v>
+      </c>
+      <c r="H51">
+        <v>8</v>
       </c>
       <c r="I51" s="1">
         <v>5</v>
@@ -2104,7 +2122,7 @@
       <c r="B54" s="6"/>
       <c r="C54" s="6">
         <f>SUM(C2:C53)</f>
-        <v>1084</v>
+        <v>1164</v>
       </c>
       <c r="D54" s="6">
         <f t="shared" ref="D54:I54" si="1">SUM(D2:D53)</f>
@@ -2124,7 +2142,7 @@
       </c>
       <c r="H54" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I54" s="6">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
did some changes to the worksheet
</commit_message>
<xml_diff>
--- a/manual/worksheet.xlsx
+++ b/manual/worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\joarbels\projects\let-me-out\manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A53C1C7-C509-E841-8E7F-FF814BB19E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292E2526-4720-4B87-AB8C-39BAE8A22572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5D3956B-3109-564E-A76F-128F28CA28C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Hours</t>
   </si>
   <si>
-    <t>TASK</t>
-  </si>
-  <si>
     <t>Research paper structure</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>Comment each others sections constructively</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Isn't it the automated thing we do everyday? So basically no time from us, but the scripts are working instead</t>
   </si>
   <si>
@@ -302,9 +296,6 @@
     <t>Gergely</t>
   </si>
   <si>
-    <t>WORKING HOUR PER MEMBER</t>
-  </si>
-  <si>
     <t>Help others: to understand networking basics and with their asks</t>
   </si>
   <si>
@@ -312,13 +303,19 @@
   </si>
   <si>
     <t>Rasmus</t>
+  </si>
+  <si>
+    <t>ROUGH ESTIMATION OF WORKING HOUR PER MEMBER</t>
+  </si>
+  <si>
+    <t>TASK (Not all shown)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -771,63 +768,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA831349-0FC3-5540-B36A-3848ABED492D}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="88" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="43.69921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="69.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="6" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.69921875" customWidth="1"/>
+    <col min="10" max="10" width="16.796875" customWidth="1"/>
+    <col min="11" max="11" width="14.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="25.8">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(D2:J2)</f>
@@ -845,12 +842,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="31.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6">
         <f t="shared" ref="C3:C50" si="0">SUM(D3:J3)</f>
@@ -878,12 +875,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="31.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="6">
         <f t="shared" si="0"/>
@@ -911,12 +908,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="31.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
@@ -944,12 +941,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
@@ -967,12 +964,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
@@ -994,22 +991,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="78">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I8" s="1">
         <v>5</v>
@@ -1021,12 +1016,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="40.200000000000003">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
@@ -1044,12 +1039,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
@@ -1075,12 +1070,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="31.2">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
@@ -1108,12 +1103,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="40.200000000000003">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
@@ -1132,12 +1127,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
@@ -1158,12 +1153,12 @@
       </c>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
@@ -1183,12 +1178,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="27">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
@@ -1207,12 +1202,12 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="27">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
@@ -1228,12 +1223,12 @@
       </c>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="31.2">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6">
         <f>SUM(D17:J17)</f>
@@ -1253,12 +1248,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
@@ -1272,12 +1267,12 @@
       </c>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
@@ -1293,12 +1288,12 @@
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" ht="43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="40.200000000000003">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
@@ -1321,12 +1316,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="27">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
@@ -1344,12 +1339,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="27">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
@@ -1365,12 +1360,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="27">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
@@ -1384,12 +1379,12 @@
       </c>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="6">
         <f t="shared" si="0"/>
@@ -1409,12 +1404,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="6">
         <f t="shared" si="0"/>
@@ -1434,12 +1429,12 @@
       </c>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="46.8">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="6">
         <f t="shared" si="0"/>
@@ -1470,19 +1465,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="6">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D27" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E27" s="1">
         <v>28</v>
@@ -1495,19 +1490,19 @@
       </c>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E28" s="1">
         <v>16</v>
@@ -1521,12 +1516,12 @@
       </c>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="6">
         <f t="shared" si="0"/>
@@ -1545,12 +1540,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="6">
         <f t="shared" si="0"/>
@@ -1569,12 +1564,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="6">
         <f t="shared" si="0"/>
@@ -1596,12 +1591,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="6">
         <f t="shared" si="0"/>
@@ -1620,12 +1615,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" s="6">
         <f t="shared" si="0"/>
@@ -1641,12 +1636,12 @@
       </c>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="6">
         <f t="shared" si="0"/>
@@ -1663,12 +1658,12 @@
       </c>
       <c r="K34" s="9"/>
     </row>
-    <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="6">
         <f t="shared" si="0"/>
@@ -1682,12 +1677,12 @@
       </c>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="1:11" ht="43" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="40.200000000000003">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="6">
         <f t="shared" si="0"/>
@@ -1707,12 +1702,12 @@
       </c>
       <c r="K36" s="9"/>
     </row>
-    <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="27">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="6">
         <f t="shared" si="0"/>
@@ -1728,12 +1723,12 @@
       </c>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="6">
         <f t="shared" si="0"/>
@@ -1753,12 +1748,12 @@
       </c>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="6">
         <f t="shared" si="0"/>
@@ -1777,12 +1772,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" s="6">
         <f t="shared" si="0"/>
@@ -1801,12 +1796,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" s="6">
         <f t="shared" si="0"/>
@@ -1822,12 +1817,12 @@
       </c>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="0"/>
@@ -1841,19 +1836,19 @@
       </c>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="46.8">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" s="6">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E43" s="1">
         <v>6</v>
@@ -1877,12 +1872,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" s="6">
         <f t="shared" si="0"/>
@@ -1900,12 +1895,12 @@
       </c>
       <c r="K44" s="9"/>
     </row>
-    <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="6">
         <f t="shared" si="0"/>
@@ -1923,19 +1918,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="6">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D46" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E46" s="1">
         <v>4</v>
@@ -1948,12 +1943,12 @@
       </c>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="6">
         <f t="shared" si="0"/>
@@ -1972,12 +1967,12 @@
       </c>
       <c r="K47" s="9"/>
     </row>
-    <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C48" s="6">
         <f t="shared" si="0"/>
@@ -1993,12 +1988,12 @@
       </c>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C49" s="6">
         <f t="shared" si="0"/>
@@ -2018,12 +2013,12 @@
       </c>
       <c r="K49" s="9"/>
     </row>
-    <row r="50" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" s="6">
         <f t="shared" si="0"/>
@@ -2041,12 +2036,12 @@
       </c>
       <c r="K50" s="9"/>
     </row>
-    <row r="51" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="46.8">
       <c r="A51" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="6">
         <f>SUM(D51:J51)</f>
@@ -2077,12 +2072,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="7" customFormat="1" ht="35" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="7" customFormat="1" ht="33">
       <c r="A52" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -2096,12 +2091,12 @@
       </c>
       <c r="K52" s="10"/>
     </row>
-    <row r="53" spans="1:11" s="7" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="7" customFormat="1" ht="19.2">
       <c r="A53" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
@@ -2115,18 +2110,18 @@
       </c>
       <c r="K53" s="10"/>
     </row>
-    <row r="54" spans="1:11" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="7" customFormat="1" ht="31.2">
       <c r="A54" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="6">
         <f>SUM(C2:C53)</f>
-        <v>1164</v>
+        <v>1180</v>
       </c>
       <c r="D54" s="6">
         <f t="shared" ref="D54:I54" si="1">SUM(D2:D53)</f>
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="E54" s="6">
         <f t="shared" si="1"/>

</xml_diff>